<commit_message>
payments view was comleted
</commit_message>
<xml_diff>
--- a/app/raports/waranty_parts_XX.XX.XXXX.xlsx
+++ b/app/raports/waranty_parts_XX.XX.XXXX.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -405,21 +405,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>JUNO E1015</t>
+          <t>Elna 745</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>12345697</t>
+          <t>627970020</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>121212</t>
+          <t>797505001</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -427,65 +427,65 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>cześć 3</t>
+          <t>Needle plate</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>adsad</t>
+          <t>Nowa płytka - skorodowana lub źle wykończona</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>16</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>JANOME MB-7</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>712500078</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>771039009</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>7</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>JANOME MB-4S</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>12345697</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>123456</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>part 32</t>
+          <t>Spring</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>adsdaSA</t>
+          <t>7 szt.  Sprężyny włożone przez producenta nie zapewniają wystarczającego docisku dla rolek czujnika przez co maszyna dalej pracuje mimo braku nici.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>JUNO E1015</t>
+          <t>JANOME 990D</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>12345697</t>
+          <t>789269381</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2121233</t>
+          <t>M2042A</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -493,32 +493,32 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>the part</t>
+          <t>Motor</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>fff</t>
+          <t>Popsute uzwojenie silnika</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>JUNO E1015</t>
+          <t>JUNO E1050</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>12345697</t>
+          <t>830096302</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>121212</t>
+          <t>808505237</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -526,32 +526,32 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>xzcxscz</t>
+          <t>Printed circuit board A (unit)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>adsa</t>
+          <t>Brak prawidłowej inicjacji pracy.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>JUNO E1015</t>
+          <t>JANOME MC500E</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>121233</t>
+          <t>810014279</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>121212</t>
+          <t>843518302</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -559,32 +559,32 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>sadfa</t>
+          <t>DC Motor</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>adsad</t>
+          <t>Motor shaft and rear bushing are damaged</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>JUNO E1015</t>
+          <t>JANOME SKYLINE S3</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>12345697</t>
+          <t>710020587</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>121212</t>
+          <t>852524000+863022A03+ 863021006</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -592,32 +592,32 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>cześć 3</t>
+          <t>same situation like in December</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>broken panel inside the machines</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>JUNO E1015</t>
+          <t>JANOME 990D</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>12345697</t>
+          <t>789274986</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>121212</t>
+          <t>777502109</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -625,45 +625,1035 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>cześć 3</t>
+          <t>Machine socket (unit)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>Doesn't work</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>JANOME 990D</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>789274986</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   M2042A</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Motor (unit)</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Doesn't work</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>36</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>JANOME MC6600p</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>846635006</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>846635006</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Feed motor (unit)</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the feed motor works incorrectly </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>39</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>JANOME 744D</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>794081517</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">M2068A     </t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Motor unit</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>works incorrectly</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>40</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>JANOME DXL603</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>840124533</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>808400002</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Printed Circuit Board A</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>shows errors on the screen</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>41</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>JANOME 1200D</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>821058640</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>797604001</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Needle bar (unit)</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Needle bar has incorrectly space between needles</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>42</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>JANOME 990D</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>789272423</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>787108009</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Crank Setscrew</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>the screws were loose (2 pcs)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>43</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>JANOME 990D</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>789272423</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>785024004</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>L. looper base (2)</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the loose screws was responsible for damaged looper base </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>46</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>JUNO E1050</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>830096212</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>508638002</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Bobbin holder (unit)</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>the bobin holder was broken after few days of use..</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>47</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>JUNO E1050</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>830096212</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>808625005</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Hook race (unit)</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The hook race was has damaged surface. </t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>50</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>JANOME QXL605</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>810002853</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>808505123</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Printed Circuit Board A </t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Machine sews the different stitch than it is chosen</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>51</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>JANOME 415</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>820047949</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>043970106</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>FOOT CONTROL FOR CONTINENTAL EUROPE</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Rozrusznik nie steruje prawidłowo obrotami maszyny.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>52</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>JANOME 423S</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>840131605</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>043970106</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>FOOT CONTROL FOR CONTINENTAL EUROPE</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Rozrusznik nie steruje prawidłowo obrotami maszyny.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>53</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>JANOME TXL607</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>710014466</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>808617004</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>DC motor (unit)</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Zbyt ciasno skręcone elementy dolnego wału skutkowały zbyt dużym obciążeniem silnika co doprowadzało do przegrzewania i uszkodzenia. Silnik nie wchodzi na obroty.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>54</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>JANOME MB-7</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>712500078</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>770463302</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Printed circuit board B (unit)</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Mimo dochodzącego do urządzenia prądu maszyna nie reaguje na próby uruchomienia.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>55</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>JANOME MB-7</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>712500078</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>771503009</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Printed circuit board G (unit)</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Hafciarka po 8 godzinach pracy informuje o zerwaniu nici pomimo że do tego nie doszło.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>56</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>JANOME MC6700p</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>840125379</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>866621001</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Printed circuit board A (unit)</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>bobin winder is working all the time https://we.tl/t-VJOe1RCbEA</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>59</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>JANOME 423S</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>720304078</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>730038001</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Lower shaft gear</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Tryb napędu chwytacza zmienia swoje położenie względem mocowania.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>60</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>JANOME 393</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>721372504</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>042870308</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Foot control</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Rozrusznik nie uruchamia silnika maszyny. (Data zakupu maszyny - 10-12-2018)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>61</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>JANOME TXL607</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>630055478</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>808615002</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Bobbin winder (unit)</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Szpulownik pracuje bardzo wolno, opornie, momentami się zacina.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>62</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>JANOME AT2000D</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>831104270</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>799503005</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Lower looper (unit)</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Maszyna po niecałch 3 tygodniach użytkowania ma złamany chwytacz. Podejrzewamy wadę materiału.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>63</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>JANOME 990D</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>789268192</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>793613300</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Upper knife drive arm (unit)</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Niewłaściwy kąt prowadzenia ostrza noża.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>64</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>JANOME 990D</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>789268192</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>792603005</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Lower knife (unit)</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Niewłaściwy kąt prowadzenia ostrza noża.</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>66</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>JUNO E1019</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>520297674</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>508648304</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Motor (unit)</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Brak reakcji silnika. (Data zakupu 06.03.2017)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>67</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>JANOME SEW MINI</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>630338253</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>525037008</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gear b </t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Wada fabryczna, tryb luźno pracuje na wałku.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>68</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>JANOME SEW MINI</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>630338253</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>525621005</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DC motor </t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Silnik drgnie po wciśnięciu rozrusznika i przestaje pracować.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>69</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>JUNO E1019</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>530607796</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>508648304</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Motor</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Silnik nie reaguje.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>71</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>JANOME 1200D</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>522081969</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>797643002</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Motor (unit) 230V</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Przepalone uzwojenie silnika. (03/03/2017)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>72</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>ELNA SEW 75</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>720304220</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>043970106</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Foot control</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Drgania igielnicy pomimo zwolnienia rozrusznika nożnego.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>73</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>JANOME MB-7</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>000000000</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>770463302</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Printed circuit board B (unit)</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Płyta zakupiona 15/04/2019 po miesiącu płyta nie działa. Po uruchomieniu oświetlenie maszyny błyśnie i podświetla się panel boczny - hafciarka nie reaguje. Mamy filmik obrazujący usterkę.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>74</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>JANOME MC500E</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>740087305</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>864616007</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Thread cutter (unit)</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Źle osadzony (luźny) napęd noża.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>75</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
           <t>JUNO E1015</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>12345697</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>121212</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>cześć 3</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>asd</t>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>810002698</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>743671024</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Motor assembly (unit)</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Maszyna szyje bardzo powoli. Po kilku sekundach szycia z maszyny wydobywa się zapach spalenizny z silnika.(data zakupu 16-03-2018)</t>
         </is>
       </c>
     </row>

</xml_diff>